<commit_message>
modified members and navbar
</commit_message>
<xml_diff>
--- a/js/members/Toppa Directory.xlsx
+++ b/js/members/Toppa Directory.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="157">
   <si>
     <t>Timestamp</t>
   </si>
@@ -109,19 +109,19 @@
     <t>mattyan1726@berkeley.edu</t>
   </si>
   <si>
-    <t>CS + Applied Math</t>
+    <t>CS &amp; Applied Math</t>
   </si>
   <si>
     <t>NGO Consulting for Pandemic Professors</t>
   </si>
   <si>
-    <t>https://drive.google.com/open?id=1M1WJqb2yM3V_x85wRTQ-oN1bruDWXd3Q</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hello! I'm Matt, a sophomore majoring in CS and Applied Math. In my free time, I would like to watch YouTube, and I enjoy playing tennis, piano and skiing. </t>
-  </si>
-  <si>
-    <t>SWE, Data Analyst, still exploring</t>
+    <t>https://drive.google.com/open?id=1UKoNUE4mrsQYRmbyx1TQ85KH_-1jbMaB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hello! I am Matt, a sophomore student majoring in CS and Applied Math. I enjoy playing tennis, piano, and skiing. In my free time, I would like to watch YouTube and prob read some novel. </t>
+  </si>
+  <si>
+    <t>SWE, Data Analyst</t>
   </si>
   <si>
     <t>Matt-Yan-1.jpeg</t>
@@ -411,6 +411,78 @@
   </si>
   <si>
     <t>Stephanie-Liu-1.JPG</t>
+  </si>
+  <si>
+    <t>Kerry</t>
+  </si>
+  <si>
+    <t>Wong</t>
+  </si>
+  <si>
+    <t>kerrywong@berkeley.edu</t>
+  </si>
+  <si>
+    <t>Intended Business Administration and Data Science</t>
+  </si>
+  <si>
+    <t>Newsletter &amp; Toppa E-book</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=1yhokc7HXK3clBtITm5hHJTTmyxCvBhjb, https://drive.google.com/open?id=1rgwDfuMRaQCQiP-qpWKnQvY04ef03HFY</t>
+  </si>
+  <si>
+    <t>Hi! I'm Kerry Wong and I am a first-year hoping to major in business administration and data science. I'm from the Bay Area and I have grown up here. In the future, I hope to work in market research or data science because I'm super interested in data science and how it can be used in different careers. Outside of school, I'm passionate about social justice and equity. In my free time, I enjoy playing tennis, writing, reading, and watching movies.</t>
+  </si>
+  <si>
+    <t>I hope to work in marketing, market research, or data science.</t>
+  </si>
+  <si>
+    <t>Kerry-Wong-1.jpg</t>
+  </si>
+  <si>
+    <t>Yunhan</t>
+  </si>
+  <si>
+    <t>Jin</t>
+  </si>
+  <si>
+    <t>yunhanj@berkeley.edu</t>
+  </si>
+  <si>
+    <t>Data Science, Economics</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=1KYsB5N3wM2ekOt6RvI1JJ0x04eXhNVrG, https://drive.google.com/open?id=1IZkzS_m_-k2wBaLxB_Au53afiJ91DSNk</t>
+  </si>
+  <si>
+    <t>Hello, I am Yunhan studying Data Science and Economics, with a minor in Public Policy. I have been very interested in social sector and education work, and potentially will take it as my long-term career goal. In my free time, I like playing and watching basketball, watching Youtube videos, and listening to music.</t>
+  </si>
+  <si>
+    <t>Consulting/Data Analyst</t>
+  </si>
+  <si>
+    <t>Yunhan-Jin-1.jpg</t>
+  </si>
+  <si>
+    <t>Xuanyi (Anna)</t>
+  </si>
+  <si>
+    <t>Song</t>
+  </si>
+  <si>
+    <t>xuanyisong@berkeley.edu</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=1BfAQ4ZEyLDTeqJKXEiO0wRSpvK-QMizh, https://drive.google.com/open?id=1ke2CCFO-_JGDxyvfUwoisWVBAADaPpoS</t>
+  </si>
+  <si>
+    <t>Hi! I'm a sophomore double major in Psychology and Data Science. I'm super interested in the field of consulting and social justice. I also enjoy playing badminton, ice-curling, and cooking!</t>
+  </si>
+  <si>
+    <t>consulting/tech consulting/PM/data analysis</t>
+  </si>
+  <si>
+    <t>Xuanyi-Song-1.jpg</t>
   </si>
 </sst>
 </file>
@@ -420,10 +492,27 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yyyy h:mm:ss"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="9">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font/>
+    <font>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <color rgb="FF0000FF"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <color rgb="FF1155CC"/>
       <name val="Arial"/>
     </font>
     <font>
@@ -431,12 +520,9 @@
       <name val="Arial"/>
     </font>
     <font>
-      <color rgb="FF000000"/>
+      <u/>
+      <color rgb="FF1155CC"/>
       <name val="Arial"/>
-    </font>
-    <font>
-      <u/>
-      <color rgb="FF0000FF"/>
     </font>
     <font>
       <u/>
@@ -464,16 +550,15 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
+      <alignment shrinkToFit="0" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
@@ -487,29 +572,38 @@
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="0"/>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -730,249 +824,251 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="7" width="21.57"/>
+    <col customWidth="1" min="1" max="4" width="21.57"/>
+    <col customWidth="1" min="5" max="5" width="25.86"/>
+    <col customWidth="1" min="6" max="7" width="21.57"/>
     <col customWidth="1" min="8" max="8" width="22.57"/>
     <col customWidth="1" min="9" max="9" width="44.0"/>
-    <col customWidth="1" min="10" max="10" width="30.43"/>
+    <col customWidth="1" min="10" max="10" width="45.0"/>
     <col customWidth="1" min="11" max="16" width="21.57"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="3" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="5">
+      <c r="A2" s="4">
         <v>44119.38846581019</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="H2" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="I2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J2" s="8" t="s">
+      <c r="J2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="K2" s="3" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="5">
+      <c r="A3" s="4">
         <v>44119.453826412035</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="H3" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="I3" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="J3" s="8" t="s">
+      <c r="J3" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="K3" s="4" t="s">
+      <c r="K3" s="3" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="5">
-        <v>44119.465514166666</v>
-      </c>
-      <c r="B4" s="4" t="s">
+      <c r="A4" s="7">
+        <v>44145.51358068287</v>
+      </c>
+      <c r="B4" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="G4" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="H4" s="7" t="s">
+      <c r="H4" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="I4" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="J4" s="8" t="s">
+      <c r="J4" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="K4" s="4" t="s">
+      <c r="K4" s="3" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="5">
+      <c r="A5" s="4">
         <v>44119.47108668981</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="G5" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="H5" s="4" t="s">
+      <c r="H5" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="I5" s="2" t="s">
+      <c r="I5" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="J5" s="8" t="s">
+      <c r="J5" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="K5" s="4" t="s">
+      <c r="K5" s="3" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="5">
+      <c r="A6" s="4">
         <v>44120.59015118056</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="F6" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="G6" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="H6" s="4" t="s">
+      <c r="H6" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="I6" s="2" t="s">
+      <c r="I6" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="J6" s="8" t="s">
+      <c r="J6" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="K6" s="4" t="s">
+      <c r="K6" s="3" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="9">
+      <c r="A7" s="7">
         <v>44130.11043332176</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="D7" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="E7" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="F7" s="10" t="s">
+      <c r="F7" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="G7" s="10" t="s">
+      <c r="G7" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="H7" s="10" t="s">
+      <c r="H7" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="I7" s="11" t="s">
+      <c r="I7" s="12" t="s">
         <v>58</v>
       </c>
       <c r="J7" s="12" t="s">
@@ -981,38 +1077,38 @@
       <c r="K7" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="L7" s="10"/>
-      <c r="M7" s="10"/>
-      <c r="N7" s="10"/>
-      <c r="O7" s="10"/>
-      <c r="P7" s="10"/>
+      <c r="L7" s="14"/>
+      <c r="M7" s="14"/>
+      <c r="N7" s="14"/>
+      <c r="O7" s="14"/>
+      <c r="P7" s="14"/>
     </row>
     <row r="8">
-      <c r="A8" s="9">
+      <c r="A8" s="7">
         <v>44134.08944299769</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="D8" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="E8" s="10" t="s">
+      <c r="E8" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="F8" s="10" t="s">
+      <c r="F8" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="G8" s="10" t="s">
+      <c r="G8" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="H8" s="14" t="s">
+      <c r="H8" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="I8" s="11" t="s">
+      <c r="I8" s="12" t="s">
         <v>66</v>
       </c>
       <c r="J8" s="12" t="s">
@@ -1021,38 +1117,38 @@
       <c r="K8" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="L8" s="10"/>
-      <c r="M8" s="10"/>
-      <c r="N8" s="10"/>
-      <c r="O8" s="10"/>
-      <c r="P8" s="10"/>
+      <c r="L8" s="14"/>
+      <c r="M8" s="14"/>
+      <c r="N8" s="14"/>
+      <c r="O8" s="14"/>
+      <c r="P8" s="14"/>
     </row>
     <row r="9">
-      <c r="A9" s="9">
+      <c r="A9" s="7">
         <v>44136.55357798611</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="D9" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="E9" s="10" t="s">
+      <c r="E9" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="F9" s="10" t="s">
+      <c r="F9" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="G9" s="10" t="s">
+      <c r="G9" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="H9" s="14" t="s">
+      <c r="H9" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="I9" s="11" t="s">
+      <c r="I9" s="12" t="s">
         <v>73</v>
       </c>
       <c r="J9" s="12" t="s">
@@ -1061,38 +1157,38 @@
       <c r="K9" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="L9" s="10"/>
-      <c r="M9" s="10"/>
-      <c r="N9" s="10"/>
-      <c r="O9" s="10"/>
-      <c r="P9" s="10"/>
+      <c r="L9" s="14"/>
+      <c r="M9" s="14"/>
+      <c r="N9" s="14"/>
+      <c r="O9" s="14"/>
+      <c r="P9" s="14"/>
     </row>
     <row r="10">
-      <c r="A10" s="9">
+      <c r="A10" s="7">
         <v>44141.54130082176</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="C10" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="D10" s="10" t="s">
+      <c r="D10" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="E10" s="10" t="s">
+      <c r="E10" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="F10" s="10" t="s">
+      <c r="F10" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="G10" s="10" t="s">
+      <c r="G10" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="H10" s="10" t="s">
+      <c r="H10" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="I10" s="11" t="s">
+      <c r="I10" s="12" t="s">
         <v>82</v>
       </c>
       <c r="J10" s="12" t="s">
@@ -1101,38 +1197,38 @@
       <c r="K10" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="L10" s="10"/>
-      <c r="M10" s="10"/>
-      <c r="N10" s="10"/>
-      <c r="O10" s="10"/>
-      <c r="P10" s="10"/>
+      <c r="L10" s="11"/>
+      <c r="M10" s="14"/>
+      <c r="N10" s="14"/>
+      <c r="O10" s="14"/>
+      <c r="P10" s="14"/>
     </row>
     <row r="11">
-      <c r="A11" s="9">
+      <c r="A11" s="7">
         <v>44141.56855947917</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="C11" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="D11" s="10" t="s">
+      <c r="D11" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="E11" s="10" t="s">
+      <c r="E11" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="F11" s="10" t="s">
+      <c r="F11" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="G11" s="10" t="s">
+      <c r="G11" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="H11" s="10" t="s">
+      <c r="H11" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="I11" s="11" t="s">
+      <c r="I11" s="12" t="s">
         <v>92</v>
       </c>
       <c r="J11" s="12" t="s">
@@ -1141,38 +1237,38 @@
       <c r="K11" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="L11" s="10"/>
-      <c r="M11" s="10"/>
-      <c r="N11" s="10"/>
-      <c r="O11" s="10"/>
-      <c r="P11" s="10"/>
+      <c r="L11" s="11"/>
+      <c r="M11" s="14"/>
+      <c r="N11" s="14"/>
+      <c r="O11" s="14"/>
+      <c r="P11" s="14"/>
     </row>
     <row r="12">
-      <c r="A12" s="9">
+      <c r="A12" s="7">
         <v>44141.57226166667</v>
       </c>
-      <c r="B12" s="10" t="s">
+      <c r="B12" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="C12" s="10" t="s">
+      <c r="C12" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="10" t="s">
+      <c r="D12" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="E12" s="10" t="s">
+      <c r="E12" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="F12" s="10" t="s">
+      <c r="F12" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="G12" s="10" t="s">
+      <c r="G12" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="H12" s="10" t="s">
+      <c r="H12" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="I12" s="11" t="s">
+      <c r="I12" s="12" t="s">
         <v>99</v>
       </c>
       <c r="J12" s="12" t="s">
@@ -1181,38 +1277,38 @@
       <c r="K12" s="13" t="s">
         <v>101</v>
       </c>
-      <c r="L12" s="10"/>
-      <c r="M12" s="10"/>
-      <c r="N12" s="10"/>
-      <c r="O12" s="10"/>
-      <c r="P12" s="10"/>
+      <c r="L12" s="11"/>
+      <c r="M12" s="14"/>
+      <c r="N12" s="14"/>
+      <c r="O12" s="14"/>
+      <c r="P12" s="14"/>
     </row>
     <row r="13">
-      <c r="A13" s="9">
+      <c r="A13" s="7">
         <v>44141.58270162037</v>
       </c>
-      <c r="B13" s="10" t="s">
+      <c r="B13" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="C13" s="10" t="s">
+      <c r="C13" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="D13" s="10" t="s">
+      <c r="D13" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="E13" s="10" t="s">
+      <c r="E13" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="F13" s="10" t="s">
+      <c r="F13" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="G13" s="10" t="s">
+      <c r="G13" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="H13" s="10" t="s">
+      <c r="H13" s="11" t="s">
         <v>106</v>
       </c>
-      <c r="I13" s="11" t="s">
+      <c r="I13" s="12" t="s">
         <v>107</v>
       </c>
       <c r="J13" s="12" t="s">
@@ -1221,38 +1317,38 @@
       <c r="K13" s="13" t="s">
         <v>109</v>
       </c>
-      <c r="L13" s="10"/>
-      <c r="M13" s="10"/>
-      <c r="N13" s="10"/>
-      <c r="O13" s="10"/>
-      <c r="P13" s="10"/>
+      <c r="L13" s="11"/>
+      <c r="M13" s="14"/>
+      <c r="N13" s="14"/>
+      <c r="O13" s="14"/>
+      <c r="P13" s="14"/>
     </row>
     <row r="14">
-      <c r="A14" s="9">
+      <c r="A14" s="7">
         <v>44141.645020717595</v>
       </c>
-      <c r="B14" s="10" t="s">
+      <c r="B14" s="11" t="s">
         <v>110</v>
       </c>
-      <c r="C14" s="10" t="s">
+      <c r="C14" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="D14" s="10" t="s">
+      <c r="D14" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="E14" s="10" t="s">
+      <c r="E14" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="F14" s="10" t="s">
+      <c r="F14" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="G14" s="10" t="s">
+      <c r="G14" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="H14" s="10" t="s">
+      <c r="H14" s="11" t="s">
         <v>114</v>
       </c>
-      <c r="I14" s="11" t="s">
+      <c r="I14" s="12" t="s">
         <v>115</v>
       </c>
       <c r="J14" s="12" t="s">
@@ -1261,38 +1357,38 @@
       <c r="K14" s="13" t="s">
         <v>117</v>
       </c>
-      <c r="L14" s="10"/>
-      <c r="M14" s="10"/>
-      <c r="N14" s="10"/>
-      <c r="O14" s="10"/>
-      <c r="P14" s="10"/>
+      <c r="L14" s="11"/>
+      <c r="M14" s="14"/>
+      <c r="N14" s="14"/>
+      <c r="O14" s="14"/>
+      <c r="P14" s="14"/>
     </row>
     <row r="15">
-      <c r="A15" s="9">
+      <c r="A15" s="7">
         <v>44141.69336200232</v>
       </c>
-      <c r="B15" s="10" t="s">
+      <c r="B15" s="11" t="s">
         <v>118</v>
       </c>
-      <c r="C15" s="10" t="s">
+      <c r="C15" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="D15" s="10" t="s">
+      <c r="D15" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="E15" s="10" t="s">
+      <c r="E15" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="F15" s="10" t="s">
+      <c r="F15" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="G15" s="10" t="s">
+      <c r="G15" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="H15" s="10" t="s">
+      <c r="H15" s="11" t="s">
         <v>120</v>
       </c>
-      <c r="I15" s="11" t="s">
+      <c r="I15" s="12" t="s">
         <v>121</v>
       </c>
       <c r="J15" s="12" t="s">
@@ -1301,38 +1397,38 @@
       <c r="K15" s="13" t="s">
         <v>123</v>
       </c>
-      <c r="L15" s="10"/>
-      <c r="M15" s="10"/>
-      <c r="N15" s="10"/>
-      <c r="O15" s="10"/>
-      <c r="P15" s="10"/>
+      <c r="L15" s="11"/>
+      <c r="M15" s="11"/>
+      <c r="N15" s="11"/>
+      <c r="O15" s="14"/>
+      <c r="P15" s="14"/>
     </row>
     <row r="16">
-      <c r="A16" s="9">
+      <c r="A16" s="7">
         <v>44141.9652875926</v>
       </c>
-      <c r="B16" s="10" t="s">
+      <c r="B16" s="11" t="s">
         <v>124</v>
       </c>
-      <c r="C16" s="10" t="s">
+      <c r="C16" s="11" t="s">
         <v>125</v>
       </c>
-      <c r="D16" s="10" t="s">
+      <c r="D16" s="11" t="s">
         <v>126</v>
       </c>
-      <c r="E16" s="10" t="s">
+      <c r="E16" s="11" t="s">
         <v>127</v>
       </c>
-      <c r="F16" s="10" t="s">
+      <c r="F16" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="G16" s="10" t="s">
+      <c r="G16" s="11" t="s">
         <v>128</v>
       </c>
-      <c r="H16" s="10" t="s">
+      <c r="H16" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="I16" s="11" t="s">
+      <c r="I16" s="12" t="s">
         <v>130</v>
       </c>
       <c r="J16" s="12" t="s">
@@ -1341,371 +1437,479 @@
       <c r="K16" s="13" t="s">
         <v>132</v>
       </c>
-      <c r="L16" s="10"/>
-      <c r="M16" s="10"/>
-      <c r="N16" s="10"/>
-      <c r="O16" s="10"/>
-      <c r="P16" s="10"/>
+      <c r="L16" s="14"/>
+      <c r="M16" s="14"/>
+      <c r="N16" s="14"/>
+      <c r="O16" s="14"/>
+      <c r="P16" s="14"/>
     </row>
     <row r="17">
-      <c r="I17" s="15"/>
-      <c r="J17" s="3"/>
+      <c r="A17" s="7">
+        <v>44145.62176787037</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="F17" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="G17" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="H17" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="I17" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="J17" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="K17" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="L17" s="14"/>
+      <c r="M17" s="14"/>
+      <c r="N17" s="14"/>
+      <c r="O17" s="14"/>
+      <c r="P17" s="14"/>
     </row>
     <row r="18">
-      <c r="I18" s="15"/>
-      <c r="J18" s="3"/>
+      <c r="A18" s="7">
+        <v>44146.31756053241</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>143</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="E18" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="F18" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="G18" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="H18" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="I18" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="J18" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="K18" s="13" t="s">
+        <v>149</v>
+      </c>
+      <c r="L18" s="14"/>
+      <c r="M18" s="14"/>
+      <c r="N18" s="14"/>
+      <c r="O18" s="14"/>
+      <c r="P18" s="14"/>
     </row>
     <row r="19">
-      <c r="I19" s="15"/>
-      <c r="J19" s="3"/>
+      <c r="A19" s="7">
+        <v>44146.693440752315</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>152</v>
+      </c>
+      <c r="E19" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="F19" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="G19" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="H19" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="I19" s="12" t="s">
+        <v>154</v>
+      </c>
+      <c r="J19" s="12" t="s">
+        <v>155</v>
+      </c>
+      <c r="K19" s="13" t="s">
+        <v>156</v>
+      </c>
+      <c r="L19" s="14"/>
+      <c r="M19" s="14"/>
+      <c r="N19" s="14"/>
+      <c r="O19" s="14"/>
+      <c r="P19" s="14"/>
     </row>
     <row r="20">
-      <c r="I20" s="15"/>
-      <c r="J20" s="3"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2"/>
     </row>
     <row r="21">
-      <c r="I21" s="15"/>
-      <c r="J21" s="3"/>
+      <c r="I21" s="2"/>
+      <c r="J21" s="2"/>
     </row>
     <row r="22">
-      <c r="I22" s="15"/>
-      <c r="J22" s="3"/>
+      <c r="I22" s="2"/>
+      <c r="J22" s="2"/>
     </row>
     <row r="23">
-      <c r="I23" s="15"/>
-      <c r="J23" s="3"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="2"/>
     </row>
     <row r="24">
-      <c r="I24" s="15"/>
-      <c r="J24" s="3"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2"/>
     </row>
     <row r="25">
-      <c r="I25" s="15"/>
-      <c r="J25" s="3"/>
+      <c r="I25" s="2"/>
+      <c r="J25" s="2"/>
     </row>
     <row r="26">
-      <c r="I26" s="15"/>
-      <c r="J26" s="3"/>
+      <c r="I26" s="2"/>
+      <c r="J26" s="2"/>
     </row>
     <row r="27">
-      <c r="I27" s="15"/>
-      <c r="J27" s="3"/>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2"/>
     </row>
     <row r="28">
-      <c r="I28" s="15"/>
-      <c r="J28" s="3"/>
+      <c r="I28" s="2"/>
+      <c r="J28" s="2"/>
     </row>
     <row r="29">
-      <c r="I29" s="15"/>
-      <c r="J29" s="3"/>
+      <c r="I29" s="2"/>
+      <c r="J29" s="2"/>
     </row>
     <row r="30">
-      <c r="I30" s="15"/>
-      <c r="J30" s="3"/>
+      <c r="I30" s="2"/>
+      <c r="J30" s="2"/>
     </row>
     <row r="31">
-      <c r="I31" s="15"/>
-      <c r="J31" s="3"/>
+      <c r="I31" s="2"/>
+      <c r="J31" s="2"/>
     </row>
     <row r="32">
-      <c r="I32" s="15"/>
-      <c r="J32" s="3"/>
+      <c r="I32" s="2"/>
+      <c r="J32" s="2"/>
     </row>
     <row r="33">
-      <c r="I33" s="15"/>
-      <c r="J33" s="3"/>
+      <c r="I33" s="2"/>
+      <c r="J33" s="2"/>
     </row>
     <row r="34">
-      <c r="I34" s="15"/>
-      <c r="J34" s="3"/>
+      <c r="I34" s="2"/>
+      <c r="J34" s="2"/>
     </row>
     <row r="35">
-      <c r="I35" s="15"/>
-      <c r="J35" s="3"/>
+      <c r="I35" s="2"/>
+      <c r="J35" s="2"/>
     </row>
     <row r="36">
-      <c r="I36" s="15"/>
-      <c r="J36" s="3"/>
+      <c r="I36" s="2"/>
+      <c r="J36" s="2"/>
     </row>
     <row r="37">
-      <c r="I37" s="15"/>
-      <c r="J37" s="3"/>
+      <c r="I37" s="2"/>
+      <c r="J37" s="2"/>
     </row>
     <row r="38">
-      <c r="I38" s="15"/>
-      <c r="J38" s="3"/>
+      <c r="I38" s="2"/>
+      <c r="J38" s="2"/>
     </row>
     <row r="39">
-      <c r="I39" s="15"/>
-      <c r="J39" s="3"/>
+      <c r="I39" s="2"/>
+      <c r="J39" s="2"/>
     </row>
     <row r="40">
-      <c r="I40" s="15"/>
-      <c r="J40" s="3"/>
+      <c r="I40" s="2"/>
+      <c r="J40" s="2"/>
     </row>
     <row r="41">
-      <c r="I41" s="15"/>
-      <c r="J41" s="3"/>
+      <c r="I41" s="2"/>
+      <c r="J41" s="2"/>
     </row>
     <row r="42">
-      <c r="I42" s="15"/>
-      <c r="J42" s="3"/>
+      <c r="I42" s="2"/>
+      <c r="J42" s="2"/>
     </row>
     <row r="43">
-      <c r="I43" s="15"/>
-      <c r="J43" s="3"/>
+      <c r="I43" s="2"/>
+      <c r="J43" s="2"/>
     </row>
     <row r="44">
-      <c r="I44" s="15"/>
-      <c r="J44" s="3"/>
+      <c r="I44" s="2"/>
+      <c r="J44" s="2"/>
     </row>
     <row r="45">
-      <c r="I45" s="15"/>
-      <c r="J45" s="3"/>
+      <c r="I45" s="2"/>
+      <c r="J45" s="2"/>
     </row>
     <row r="46">
-      <c r="I46" s="15"/>
-      <c r="J46" s="3"/>
+      <c r="I46" s="2"/>
+      <c r="J46" s="2"/>
     </row>
     <row r="47">
-      <c r="I47" s="15"/>
-      <c r="J47" s="3"/>
+      <c r="I47" s="2"/>
+      <c r="J47" s="2"/>
     </row>
     <row r="48">
-      <c r="I48" s="15"/>
-      <c r="J48" s="3"/>
+      <c r="I48" s="2"/>
+      <c r="J48" s="2"/>
     </row>
     <row r="49">
-      <c r="I49" s="15"/>
-      <c r="J49" s="3"/>
+      <c r="I49" s="2"/>
+      <c r="J49" s="2"/>
     </row>
     <row r="50">
-      <c r="I50" s="15"/>
-      <c r="J50" s="3"/>
+      <c r="I50" s="2"/>
+      <c r="J50" s="2"/>
     </row>
     <row r="51">
-      <c r="I51" s="15"/>
-      <c r="J51" s="3"/>
+      <c r="I51" s="2"/>
+      <c r="J51" s="2"/>
     </row>
     <row r="52">
-      <c r="I52" s="15"/>
-      <c r="J52" s="3"/>
+      <c r="I52" s="2"/>
+      <c r="J52" s="2"/>
     </row>
     <row r="53">
-      <c r="I53" s="15"/>
-      <c r="J53" s="3"/>
+      <c r="I53" s="2"/>
+      <c r="J53" s="2"/>
     </row>
     <row r="54">
-      <c r="I54" s="15"/>
-      <c r="J54" s="3"/>
+      <c r="I54" s="2"/>
+      <c r="J54" s="2"/>
     </row>
     <row r="55">
-      <c r="I55" s="15"/>
-      <c r="J55" s="3"/>
+      <c r="I55" s="2"/>
+      <c r="J55" s="2"/>
     </row>
     <row r="56">
-      <c r="I56" s="15"/>
-      <c r="J56" s="3"/>
+      <c r="I56" s="2"/>
+      <c r="J56" s="2"/>
     </row>
     <row r="57">
-      <c r="I57" s="15"/>
-      <c r="J57" s="3"/>
+      <c r="I57" s="2"/>
+      <c r="J57" s="2"/>
     </row>
     <row r="58">
-      <c r="I58" s="15"/>
-      <c r="J58" s="3"/>
+      <c r="I58" s="2"/>
+      <c r="J58" s="2"/>
     </row>
     <row r="59">
-      <c r="I59" s="15"/>
-      <c r="J59" s="3"/>
+      <c r="I59" s="2"/>
+      <c r="J59" s="2"/>
     </row>
     <row r="60">
-      <c r="I60" s="15"/>
-      <c r="J60" s="3"/>
+      <c r="I60" s="2"/>
+      <c r="J60" s="2"/>
     </row>
     <row r="61">
-      <c r="I61" s="15"/>
-      <c r="J61" s="3"/>
+      <c r="I61" s="2"/>
+      <c r="J61" s="2"/>
     </row>
     <row r="62">
-      <c r="I62" s="15"/>
-      <c r="J62" s="3"/>
+      <c r="I62" s="2"/>
+      <c r="J62" s="2"/>
     </row>
     <row r="63">
-      <c r="I63" s="15"/>
-      <c r="J63" s="3"/>
+      <c r="I63" s="2"/>
+      <c r="J63" s="2"/>
     </row>
     <row r="64">
-      <c r="I64" s="15"/>
-      <c r="J64" s="3"/>
+      <c r="I64" s="2"/>
+      <c r="J64" s="2"/>
     </row>
     <row r="65">
-      <c r="I65" s="15"/>
-      <c r="J65" s="3"/>
+      <c r="I65" s="2"/>
+      <c r="J65" s="2"/>
     </row>
     <row r="66">
-      <c r="I66" s="15"/>
-      <c r="J66" s="3"/>
+      <c r="I66" s="2"/>
+      <c r="J66" s="2"/>
     </row>
     <row r="67">
-      <c r="I67" s="15"/>
-      <c r="J67" s="3"/>
+      <c r="I67" s="2"/>
+      <c r="J67" s="2"/>
     </row>
     <row r="68">
-      <c r="I68" s="15"/>
-      <c r="J68" s="3"/>
+      <c r="I68" s="2"/>
+      <c r="J68" s="2"/>
     </row>
     <row r="69">
-      <c r="I69" s="15"/>
-      <c r="J69" s="3"/>
+      <c r="I69" s="2"/>
+      <c r="J69" s="2"/>
     </row>
     <row r="70">
-      <c r="I70" s="15"/>
-      <c r="J70" s="3"/>
+      <c r="I70" s="2"/>
+      <c r="J70" s="2"/>
     </row>
     <row r="71">
-      <c r="I71" s="15"/>
-      <c r="J71" s="3"/>
+      <c r="I71" s="2"/>
+      <c r="J71" s="2"/>
     </row>
     <row r="72">
-      <c r="I72" s="15"/>
-      <c r="J72" s="3"/>
+      <c r="I72" s="2"/>
+      <c r="J72" s="2"/>
     </row>
     <row r="73">
-      <c r="I73" s="15"/>
-      <c r="J73" s="3"/>
+      <c r="I73" s="2"/>
+      <c r="J73" s="2"/>
     </row>
     <row r="74">
-      <c r="I74" s="15"/>
-      <c r="J74" s="3"/>
+      <c r="I74" s="2"/>
+      <c r="J74" s="2"/>
     </row>
     <row r="75">
-      <c r="I75" s="15"/>
-      <c r="J75" s="3"/>
+      <c r="I75" s="2"/>
+      <c r="J75" s="2"/>
     </row>
     <row r="76">
-      <c r="I76" s="15"/>
-      <c r="J76" s="3"/>
+      <c r="I76" s="2"/>
+      <c r="J76" s="2"/>
     </row>
     <row r="77">
-      <c r="I77" s="15"/>
-      <c r="J77" s="3"/>
+      <c r="I77" s="2"/>
+      <c r="J77" s="2"/>
     </row>
     <row r="78">
-      <c r="I78" s="15"/>
-      <c r="J78" s="3"/>
+      <c r="I78" s="2"/>
+      <c r="J78" s="2"/>
     </row>
     <row r="79">
-      <c r="I79" s="15"/>
-      <c r="J79" s="3"/>
+      <c r="I79" s="2"/>
+      <c r="J79" s="2"/>
     </row>
     <row r="80">
-      <c r="I80" s="15"/>
-      <c r="J80" s="3"/>
+      <c r="I80" s="2"/>
+      <c r="J80" s="2"/>
     </row>
     <row r="81">
-      <c r="I81" s="15"/>
-      <c r="J81" s="3"/>
+      <c r="I81" s="2"/>
+      <c r="J81" s="2"/>
     </row>
     <row r="82">
-      <c r="I82" s="15"/>
-      <c r="J82" s="3"/>
+      <c r="I82" s="2"/>
+      <c r="J82" s="2"/>
     </row>
     <row r="83">
-      <c r="I83" s="15"/>
-      <c r="J83" s="3"/>
+      <c r="I83" s="2"/>
+      <c r="J83" s="2"/>
     </row>
     <row r="84">
-      <c r="I84" s="15"/>
-      <c r="J84" s="3"/>
+      <c r="I84" s="2"/>
+      <c r="J84" s="2"/>
     </row>
     <row r="85">
-      <c r="I85" s="15"/>
-      <c r="J85" s="3"/>
+      <c r="I85" s="2"/>
+      <c r="J85" s="2"/>
     </row>
     <row r="86">
-      <c r="I86" s="15"/>
-      <c r="J86" s="3"/>
+      <c r="I86" s="2"/>
+      <c r="J86" s="2"/>
     </row>
     <row r="87">
-      <c r="I87" s="15"/>
-      <c r="J87" s="3"/>
+      <c r="I87" s="2"/>
+      <c r="J87" s="2"/>
     </row>
     <row r="88">
-      <c r="I88" s="15"/>
-      <c r="J88" s="3"/>
+      <c r="I88" s="2"/>
+      <c r="J88" s="2"/>
     </row>
     <row r="89">
-      <c r="I89" s="15"/>
-      <c r="J89" s="3"/>
+      <c r="I89" s="2"/>
+      <c r="J89" s="2"/>
     </row>
     <row r="90">
-      <c r="I90" s="15"/>
-      <c r="J90" s="3"/>
+      <c r="I90" s="2"/>
+      <c r="J90" s="2"/>
     </row>
     <row r="91">
-      <c r="I91" s="15"/>
-      <c r="J91" s="3"/>
+      <c r="I91" s="2"/>
+      <c r="J91" s="2"/>
     </row>
     <row r="92">
-      <c r="I92" s="15"/>
-      <c r="J92" s="3"/>
+      <c r="I92" s="2"/>
+      <c r="J92" s="2"/>
     </row>
     <row r="93">
-      <c r="I93" s="15"/>
-      <c r="J93" s="3"/>
+      <c r="I93" s="2"/>
+      <c r="J93" s="2"/>
     </row>
     <row r="94">
-      <c r="I94" s="15"/>
-      <c r="J94" s="3"/>
+      <c r="I94" s="2"/>
+      <c r="J94" s="2"/>
     </row>
     <row r="95">
-      <c r="I95" s="15"/>
-      <c r="J95" s="3"/>
+      <c r="I95" s="2"/>
+      <c r="J95" s="2"/>
     </row>
     <row r="96">
-      <c r="I96" s="15"/>
-      <c r="J96" s="3"/>
+      <c r="I96" s="2"/>
+      <c r="J96" s="2"/>
     </row>
     <row r="97">
-      <c r="I97" s="15"/>
-      <c r="J97" s="3"/>
+      <c r="I97" s="2"/>
+      <c r="J97" s="2"/>
     </row>
     <row r="98">
-      <c r="I98" s="15"/>
-      <c r="J98" s="3"/>
+      <c r="I98" s="2"/>
+      <c r="J98" s="2"/>
     </row>
     <row r="99">
-      <c r="I99" s="15"/>
-      <c r="J99" s="3"/>
+      <c r="I99" s="2"/>
+      <c r="J99" s="2"/>
     </row>
     <row r="100">
-      <c r="I100" s="15"/>
-      <c r="J100" s="3"/>
+      <c r="I100" s="2"/>
+      <c r="J100" s="2"/>
     </row>
     <row r="101">
-      <c r="I101" s="15"/>
-      <c r="J101" s="3"/>
+      <c r="I101" s="2"/>
+      <c r="J101" s="2"/>
     </row>
     <row r="102">
-      <c r="I102" s="15"/>
-      <c r="J102" s="3"/>
+      <c r="I102" s="2"/>
+      <c r="J102" s="2"/>
     </row>
     <row r="103">
-      <c r="I103" s="15"/>
-      <c r="J103" s="3"/>
+      <c r="I103" s="2"/>
+      <c r="J103" s="2"/>
     </row>
     <row r="104">
-      <c r="I104" s="15"/>
-      <c r="J104" s="3"/>
+      <c r="I104" s="2"/>
+      <c r="J104" s="2"/>
     </row>
     <row r="105">
-      <c r="I105" s="15"/>
-      <c r="J105" s="3"/>
+      <c r="I105" s="2"/>
+      <c r="J105" s="2"/>
     </row>
     <row r="106">
-      <c r="I106" s="15"/>
-      <c r="J106" s="3"/>
+      <c r="I106" s="2"/>
+      <c r="J106" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>